<commit_message>
Add doc- finish init S-T RC4
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MYSCHOOL\MHUD\Second Phase\SecondProject-RC4-A51\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MYSCHOOL\MHUD\Second Phase\SecondProject-RC4-A51\SecondPhase-MHUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD984BC-4CAB-4816-9C00-35F59E86FA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D5D5CF-1B92-4010-802D-23B9727D7410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{9C288242-62A2-402E-81E6-4A86706B6A60}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Second Phase</t>
   </si>
@@ -104,13 +104,22 @@
     <t>Convert to binary</t>
   </si>
   <si>
-    <t>2.3.2</t>
-  </si>
-  <si>
-    <t>Swap</t>
-  </si>
-  <si>
     <t>Excute</t>
+  </si>
+  <si>
+    <t>Dau</t>
+  </si>
+  <si>
+    <t>2  day</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
+    <t>Truong</t>
   </si>
 </sst>
 </file>
@@ -177,14 +186,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -192,6 +195,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18343F25-7135-40EC-89F8-C3B4ACC8B5A6}">
   <dimension ref="A2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,20 +529,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -552,20 +562,20 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -574,6 +584,12 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -582,6 +598,12 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -590,6 +612,12 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -598,126 +626,163 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>2.1</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="6"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8">
+        <v>44293</v>
+      </c>
+      <c r="E11" s="8">
+        <v>44293</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8">
+        <v>44293</v>
+      </c>
+      <c r="E12" s="8">
+        <v>44293</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2.4</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>